<commit_message>
fixed motor efficiency glitch and added more mores and fuelcells
</commit_message>
<xml_diff>
--- a/Simulation/FC List.xlsx
+++ b/Simulation/FC List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>FC Name</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>HalfBallard</t>
+  </si>
+  <si>
+    <t>Ballard22</t>
+  </si>
+  <si>
+    <t>Ballard21</t>
+  </si>
+  <si>
+    <t>Ballard24</t>
+  </si>
+  <si>
+    <t>Ballard25</t>
   </si>
 </sst>
 </file>
@@ -397,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,10 +450,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>145</v>
@@ -461,10 +473,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>145</v>
@@ -479,6 +491,98 @@
         <v>0.04</v>
       </c>
       <c r="G3">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>145</v>
+      </c>
+      <c r="D4">
+        <v>0.36</v>
+      </c>
+      <c r="E4">
+        <v>0.45</v>
+      </c>
+      <c r="F4">
+        <v>0.04</v>
+      </c>
+      <c r="G4">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>145</v>
+      </c>
+      <c r="D5">
+        <v>0.36</v>
+      </c>
+      <c r="E5">
+        <v>0.45</v>
+      </c>
+      <c r="F5">
+        <v>0.04</v>
+      </c>
+      <c r="G5">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>145</v>
+      </c>
+      <c r="D6">
+        <v>0.36</v>
+      </c>
+      <c r="E6">
+        <v>0.45</v>
+      </c>
+      <c r="F6">
+        <v>0.04</v>
+      </c>
+      <c r="G6">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>46</v>
+      </c>
+      <c r="C8">
+        <v>145</v>
+      </c>
+      <c r="D8">
+        <v>0.36</v>
+      </c>
+      <c r="E8">
+        <v>0.45</v>
+      </c>
+      <c r="F8">
+        <v>0.04</v>
+      </c>
+      <c r="G8">
         <v>1.02</v>
       </c>
     </row>

</xml_diff>

<commit_message>
buck converter throttle implimented
</commit_message>
<xml_diff>
--- a/Simulation/FC List.xlsx
+++ b/Simulation/FC List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>FC Name</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>20Ballard</t>
-  </si>
-  <si>
-    <t>13Ballard</t>
   </si>
   <si>
     <t>18Ballard</t>
@@ -403,9 +400,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -442,10 +441,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>145</v>
@@ -465,7 +464,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>18</v>
@@ -506,29 +505,6 @@
         <v>0.04</v>
       </c>
       <c r="G4">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>28</v>
-      </c>
-      <c r="C5">
-        <v>145</v>
-      </c>
-      <c r="D5">
-        <v>0.36</v>
-      </c>
-      <c r="E5">
-        <v>0.45</v>
-      </c>
-      <c r="F5">
-        <v>0.04</v>
-      </c>
-      <c r="G5">
         <v>1.02</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initial Torque boost speed control code
</commit_message>
<xml_diff>
--- a/Simulation/FC List.xlsx
+++ b/Simulation/FC List.xlsx
@@ -400,20 +400,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.75" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="9.75" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="6" max="6" width="23.25" customWidth="1"/>
+    <col min="7" max="7" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -462,29 +462,6 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>145</v>
-      </c>
-      <c r="D3">
-        <v>0.36</v>
-      </c>
-      <c r="E3">
-        <v>0.45</v>
-      </c>
-      <c r="F3">
-        <v>0.04</v>
-      </c>
-      <c r="G3">
-        <v>1.02</v>
-      </c>
-    </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
@@ -505,6 +482,29 @@
         <v>0.04</v>
       </c>
       <c r="G4">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>145</v>
+      </c>
+      <c r="D5">
+        <v>0.36</v>
+      </c>
+      <c r="E5">
+        <v>0.45</v>
+      </c>
+      <c r="F5">
+        <v>0.04</v>
+      </c>
+      <c r="G5">
         <v>1.02</v>
       </c>
     </row>

</xml_diff>